<commit_message>
update anh tuan bg
</commit_message>
<xml_diff>
--- a/5. WS/1. Bộ phận bảo hành/1. Thực hiện sửa chữa bảo hành/nam2022/Thang11/2.XulyBH/XLBH2211_AnhTuanBG.xlsx
+++ b/5. WS/1. Bộ phận bảo hành/1. Thực hiện sửa chữa bảo hành/nam2022/Thang11/2.XulyBH/XLBH2211_AnhTuanBG.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="95">
   <si>
     <t>STT</t>
   </si>
@@ -313,6 +313,9 @@
   </si>
   <si>
     <t>Thiết bị không chốt GPS</t>
+  </si>
+  <si>
+    <t>Xử lý lại connecter cấp nguồn module GPS</t>
   </si>
 </sst>
 </file>
@@ -1066,8 +1069,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X115"/>
   <sheetViews>
-    <sheetView showZeros="0" tabSelected="1" topLeftCell="L1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="Q15" sqref="Q15"/>
+    <sheetView showZeros="0" tabSelected="1" topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1294,7 +1297,9 @@
         <v>62</v>
       </c>
       <c r="H6" s="62"/>
-      <c r="I6" s="58"/>
+      <c r="I6" s="58" t="s">
+        <v>81</v>
+      </c>
       <c r="J6" s="59" t="s">
         <v>93</v>
       </c>
@@ -1475,14 +1480,22 @@
       <c r="L9" s="59" t="s">
         <v>77</v>
       </c>
-      <c r="M9" s="60"/>
+      <c r="M9" s="60" t="s">
+        <v>94</v>
+      </c>
       <c r="N9" s="59"/>
-      <c r="O9" s="59"/>
+      <c r="O9" s="59" t="s">
+        <v>79</v>
+      </c>
       <c r="P9" s="60" t="s">
         <v>80</v>
       </c>
-      <c r="Q9" s="59"/>
-      <c r="R9" s="61"/>
+      <c r="Q9" s="59" t="s">
+        <v>18</v>
+      </c>
+      <c r="R9" s="61" t="s">
+        <v>31</v>
+      </c>
       <c r="S9" s="64"/>
       <c r="T9" s="55"/>
       <c r="U9" s="76"/>
@@ -1640,7 +1653,9 @@
         <v>78</v>
       </c>
       <c r="N12" s="59"/>
-      <c r="O12" s="59"/>
+      <c r="O12" s="59" t="s">
+        <v>79</v>
+      </c>
       <c r="P12" s="60" t="s">
         <v>80</v>
       </c>
@@ -1921,7 +1936,7 @@
       </c>
       <c r="V21" s="9">
         <f>COUNTIF($Q$6:$Q$51,"PC")</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="W21" s="13"/>
     </row>
@@ -2166,7 +2181,7 @@
       </c>
       <c r="V29" s="9">
         <f>COUNTIF($R$6:$R$51,"*NG*")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W29" s="13"/>
     </row>
@@ -2422,7 +2437,7 @@
       </c>
       <c r="V37" s="9">
         <f>SUM(V26:V36)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="W37" s="13"/>
     </row>

</xml_diff>

<commit_message>
update anhtuanbg + qmaps
</commit_message>
<xml_diff>
--- a/5. WS/1. Bộ phận bảo hành/1. Thực hiện sửa chữa bảo hành/nam2022/Thang11/2.XulyBH/XLBH2211_AnhTuanBG.xlsx
+++ b/5. WS/1. Bộ phận bảo hành/1. Thực hiện sửa chữa bảo hành/nam2022/Thang11/2.XulyBH/XLBH2211_AnhTuanBG.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="98">
   <si>
     <t>STT</t>
   </si>
@@ -316,6 +316,15 @@
   </si>
   <si>
     <t>Xử lý lại connecter cấp nguồn module GPS</t>
+  </si>
+  <si>
+    <t>WP21120135S00443/0032002D2E</t>
+  </si>
+  <si>
+    <t>WP21120135S02689/003200264A</t>
+  </si>
+  <si>
+    <t>Thiết bị hoạt động bình thường</t>
   </si>
 </sst>
 </file>
@@ -718,6 +727,30 @@
     <xf numFmtId="1" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -735,30 +768,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1069,8 +1078,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X115"/>
   <sheetViews>
-    <sheetView showZeros="0" tabSelected="1" topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView showZeros="0" tabSelected="1" topLeftCell="L1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="S17" sqref="S17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1102,41 +1111,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="68"/>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="68"/>
-      <c r="J1" s="68"/>
-      <c r="K1" s="68"/>
-      <c r="L1" s="68"/>
-      <c r="M1" s="68"/>
-      <c r="N1" s="68"/>
-      <c r="O1" s="68"/>
-      <c r="P1" s="68"/>
-      <c r="Q1" s="68"/>
-      <c r="R1" s="68"/>
-      <c r="S1" s="68"/>
-      <c r="T1" s="68"/>
-      <c r="U1" s="68"/>
-      <c r="V1" s="68"/>
+      <c r="A1" s="76"/>
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
+      <c r="I1" s="76"/>
+      <c r="J1" s="76"/>
+      <c r="K1" s="76"/>
+      <c r="L1" s="76"/>
+      <c r="M1" s="76"/>
+      <c r="N1" s="76"/>
+      <c r="O1" s="76"/>
+      <c r="P1" s="76"/>
+      <c r="Q1" s="76"/>
+      <c r="R1" s="76"/>
+      <c r="S1" s="76"/>
+      <c r="T1" s="76"/>
+      <c r="U1" s="76"/>
+      <c r="V1" s="76"/>
       <c r="W1" s="44"/>
     </row>
     <row r="2" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="69" t="s">
+      <c r="A2" s="77" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="71" t="s">
+      <c r="B2" s="78"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="79" t="s">
         <v>63</v>
       </c>
-      <c r="F2" s="71"/>
+      <c r="F2" s="79"/>
       <c r="G2" s="4"/>
       <c r="H2" s="20"/>
       <c r="I2" s="48"/>
@@ -1181,58 +1190,58 @@
       <c r="W3" s="26"/>
     </row>
     <row r="4" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="72" t="s">
+      <c r="A4" s="80" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="67" t="s">
+      <c r="B4" s="75" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="67"/>
-      <c r="D4" s="67"/>
-      <c r="E4" s="67"/>
-      <c r="F4" s="67"/>
-      <c r="G4" s="67"/>
-      <c r="H4" s="67"/>
-      <c r="I4" s="67"/>
-      <c r="J4" s="67" t="s">
+      <c r="C4" s="75"/>
+      <c r="D4" s="75"/>
+      <c r="E4" s="75"/>
+      <c r="F4" s="75"/>
+      <c r="G4" s="75"/>
+      <c r="H4" s="75"/>
+      <c r="I4" s="75"/>
+      <c r="J4" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="K4" s="67" t="s">
+      <c r="K4" s="75" t="s">
         <v>11</v>
       </c>
-      <c r="L4" s="67"/>
-      <c r="M4" s="73" t="s">
+      <c r="L4" s="75"/>
+      <c r="M4" s="72" t="s">
         <v>42</v>
       </c>
-      <c r="N4" s="73" t="s">
+      <c r="N4" s="72" t="s">
         <v>10</v>
       </c>
-      <c r="O4" s="73" t="s">
+      <c r="O4" s="72" t="s">
         <v>7</v>
       </c>
-      <c r="P4" s="78" t="s">
+      <c r="P4" s="70" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="73" t="s">
+      <c r="Q4" s="72" t="s">
         <v>39</v>
       </c>
-      <c r="R4" s="73" t="s">
+      <c r="R4" s="72" t="s">
         <v>53</v>
       </c>
-      <c r="S4" s="80" t="s">
+      <c r="S4" s="74" t="s">
         <v>54</v>
       </c>
       <c r="T4" s="26"/>
-      <c r="U4" s="67" t="s">
+      <c r="U4" s="75" t="s">
         <v>39</v>
       </c>
-      <c r="V4" s="67" t="s">
+      <c r="V4" s="75" t="s">
         <v>53</v>
       </c>
       <c r="W4" s="45"/>
     </row>
     <row r="5" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="72"/>
+      <c r="A5" s="80"/>
       <c r="B5" s="56" t="s">
         <v>1</v>
       </c>
@@ -1257,23 +1266,23 @@
       <c r="I5" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="67"/>
+      <c r="J5" s="75"/>
       <c r="K5" s="56" t="s">
         <v>12</v>
       </c>
       <c r="L5" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="M5" s="74"/>
-      <c r="N5" s="74"/>
-      <c r="O5" s="74"/>
-      <c r="P5" s="79"/>
-      <c r="Q5" s="74"/>
-      <c r="R5" s="74"/>
-      <c r="S5" s="80"/>
+      <c r="M5" s="73"/>
+      <c r="N5" s="73"/>
+      <c r="O5" s="73"/>
+      <c r="P5" s="71"/>
+      <c r="Q5" s="73"/>
+      <c r="R5" s="73"/>
+      <c r="S5" s="74"/>
       <c r="T5" s="26"/>
-      <c r="U5" s="67"/>
-      <c r="V5" s="67"/>
+      <c r="U5" s="75"/>
+      <c r="V5" s="75"/>
       <c r="W5" s="45"/>
     </row>
     <row r="6" spans="1:23" s="11" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1283,7 +1292,9 @@
       <c r="B6" s="57">
         <v>44870</v>
       </c>
-      <c r="C6" s="57"/>
+      <c r="C6" s="57">
+        <v>44876</v>
+      </c>
       <c r="D6" s="65" t="s">
         <v>64</v>
       </c>
@@ -1327,7 +1338,7 @@
       </c>
       <c r="S6" s="64"/>
       <c r="T6" s="55"/>
-      <c r="U6" s="75" t="s">
+      <c r="U6" s="67" t="s">
         <v>18</v>
       </c>
       <c r="V6" s="3" t="s">
@@ -1342,7 +1353,9 @@
       <c r="B7" s="57">
         <v>44870</v>
       </c>
-      <c r="C7" s="57"/>
+      <c r="C7" s="57">
+        <v>44876</v>
+      </c>
       <c r="D7" s="65" t="s">
         <v>64</v>
       </c>
@@ -1355,7 +1368,9 @@
       <c r="G7" s="65" t="s">
         <v>62</v>
       </c>
-      <c r="H7" s="62"/>
+      <c r="H7" s="62" t="s">
+        <v>95</v>
+      </c>
       <c r="I7" s="58" t="s">
         <v>81</v>
       </c>
@@ -1384,7 +1399,7 @@
       </c>
       <c r="S7" s="64"/>
       <c r="T7" s="55"/>
-      <c r="U7" s="76"/>
+      <c r="U7" s="68"/>
       <c r="V7" s="3" t="s">
         <v>35</v>
       </c>
@@ -1397,7 +1412,9 @@
       <c r="B8" s="57">
         <v>44870</v>
       </c>
-      <c r="C8" s="57"/>
+      <c r="C8" s="57">
+        <v>44876</v>
+      </c>
       <c r="D8" s="65" t="s">
         <v>64</v>
       </c>
@@ -1441,7 +1458,7 @@
       </c>
       <c r="S8" s="64"/>
       <c r="T8" s="55"/>
-      <c r="U8" s="76"/>
+      <c r="U8" s="68"/>
       <c r="V8" s="3" t="s">
         <v>21</v>
       </c>
@@ -1454,7 +1471,9 @@
       <c r="B9" s="57">
         <v>44870</v>
       </c>
-      <c r="C9" s="57"/>
+      <c r="C9" s="57">
+        <v>44876</v>
+      </c>
       <c r="D9" s="65" t="s">
         <v>64</v>
       </c>
@@ -1498,7 +1517,7 @@
       </c>
       <c r="S9" s="64"/>
       <c r="T9" s="55"/>
-      <c r="U9" s="76"/>
+      <c r="U9" s="68"/>
       <c r="V9" s="3" t="s">
         <v>51</v>
       </c>
@@ -1511,7 +1530,9 @@
       <c r="B10" s="57">
         <v>44870</v>
       </c>
-      <c r="C10" s="57"/>
+      <c r="C10" s="57">
+        <v>44876</v>
+      </c>
       <c r="D10" s="65" t="s">
         <v>64</v>
       </c>
@@ -1524,7 +1545,9 @@
       <c r="G10" s="65" t="s">
         <v>62</v>
       </c>
-      <c r="H10" s="62"/>
+      <c r="H10" s="62" t="s">
+        <v>96</v>
+      </c>
       <c r="I10" s="58" t="s">
         <v>81</v>
       </c>
@@ -1555,7 +1578,7 @@
       </c>
       <c r="S10" s="64"/>
       <c r="T10" s="55"/>
-      <c r="U10" s="76"/>
+      <c r="U10" s="68"/>
       <c r="V10" s="3" t="s">
         <v>31</v>
       </c>
@@ -1568,7 +1591,9 @@
       <c r="B11" s="57">
         <v>44870</v>
       </c>
-      <c r="C11" s="57"/>
+      <c r="C11" s="57">
+        <v>44876</v>
+      </c>
       <c r="D11" s="65" t="s">
         <v>64</v>
       </c>
@@ -1612,7 +1637,7 @@
       </c>
       <c r="S11" s="64"/>
       <c r="T11" s="55"/>
-      <c r="U11" s="76"/>
+      <c r="U11" s="68"/>
       <c r="V11" s="3" t="s">
         <v>30</v>
       </c>
@@ -1625,7 +1650,9 @@
       <c r="B12" s="57">
         <v>44870</v>
       </c>
-      <c r="C12" s="57"/>
+      <c r="C12" s="57">
+        <v>44876</v>
+      </c>
       <c r="D12" s="65" t="s">
         <v>64</v>
       </c>
@@ -1642,7 +1669,9 @@
       <c r="I12" s="58" t="s">
         <v>81</v>
       </c>
-      <c r="J12" s="59"/>
+      <c r="J12" s="59" t="s">
+        <v>97</v>
+      </c>
       <c r="K12" s="59" t="s">
         <v>75</v>
       </c>
@@ -1667,7 +1696,7 @@
       </c>
       <c r="S12" s="64"/>
       <c r="T12" s="55"/>
-      <c r="U12" s="75" t="s">
+      <c r="U12" s="67" t="s">
         <v>19</v>
       </c>
       <c r="V12" s="3" t="s">
@@ -1698,7 +1727,7 @@
       <c r="R13" s="61"/>
       <c r="S13" s="64"/>
       <c r="T13" s="55"/>
-      <c r="U13" s="76"/>
+      <c r="U13" s="68"/>
       <c r="V13" s="3" t="s">
         <v>37</v>
       </c>
@@ -1727,7 +1756,7 @@
       <c r="R14" s="61"/>
       <c r="S14" s="64"/>
       <c r="T14" s="55"/>
-      <c r="U14" s="76"/>
+      <c r="U14" s="68"/>
       <c r="V14" s="3" t="s">
         <v>36</v>
       </c>
@@ -1756,7 +1785,7 @@
       <c r="R15" s="61"/>
       <c r="S15" s="64"/>
       <c r="T15" s="13"/>
-      <c r="U15" s="76"/>
+      <c r="U15" s="68"/>
       <c r="V15" s="3" t="s">
         <v>24</v>
       </c>
@@ -1785,7 +1814,7 @@
       <c r="R16" s="61"/>
       <c r="S16" s="64"/>
       <c r="T16" s="13"/>
-      <c r="U16" s="77"/>
+      <c r="U16" s="69"/>
       <c r="V16" s="3" t="s">
         <v>25</v>
       </c>
@@ -3502,13 +3531,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="U6:U11"/>
-    <mergeCell ref="U12:U16"/>
-    <mergeCell ref="P4:P5"/>
-    <mergeCell ref="Q4:Q5"/>
-    <mergeCell ref="R4:R5"/>
-    <mergeCell ref="S4:S5"/>
-    <mergeCell ref="U4:U5"/>
     <mergeCell ref="V4:V5"/>
     <mergeCell ref="A1:V1"/>
     <mergeCell ref="A2:D2"/>
@@ -3520,6 +3542,13 @@
     <mergeCell ref="M4:M5"/>
     <mergeCell ref="N4:N5"/>
     <mergeCell ref="O4:O5"/>
+    <mergeCell ref="U6:U11"/>
+    <mergeCell ref="U12:U16"/>
+    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="Q4:Q5"/>
+    <mergeCell ref="R4:R5"/>
+    <mergeCell ref="S4:S5"/>
+    <mergeCell ref="U4:U5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3563,41 +3592,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="68"/>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="68"/>
-      <c r="J1" s="68"/>
-      <c r="K1" s="68"/>
-      <c r="L1" s="68"/>
-      <c r="M1" s="68"/>
-      <c r="N1" s="68"/>
-      <c r="O1" s="68"/>
-      <c r="P1" s="68"/>
-      <c r="Q1" s="68"/>
-      <c r="R1" s="68"/>
-      <c r="S1" s="68"/>
-      <c r="T1" s="68"/>
-      <c r="U1" s="68"/>
-      <c r="V1" s="68"/>
+      <c r="A1" s="76"/>
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
+      <c r="I1" s="76"/>
+      <c r="J1" s="76"/>
+      <c r="K1" s="76"/>
+      <c r="L1" s="76"/>
+      <c r="M1" s="76"/>
+      <c r="N1" s="76"/>
+      <c r="O1" s="76"/>
+      <c r="P1" s="76"/>
+      <c r="Q1" s="76"/>
+      <c r="R1" s="76"/>
+      <c r="S1" s="76"/>
+      <c r="T1" s="76"/>
+      <c r="U1" s="76"/>
+      <c r="V1" s="76"/>
       <c r="W1" s="44"/>
     </row>
     <row r="2" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="69" t="s">
+      <c r="A2" s="77" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="71" t="s">
+      <c r="B2" s="78"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="79" t="s">
         <v>63</v>
       </c>
-      <c r="F2" s="71"/>
+      <c r="F2" s="79"/>
       <c r="G2" s="4"/>
       <c r="H2" s="20"/>
       <c r="I2" s="20"/>
@@ -3642,58 +3671,58 @@
       <c r="W3" s="26"/>
     </row>
     <row r="4" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="72" t="s">
+      <c r="A4" s="80" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="67" t="s">
+      <c r="B4" s="75" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="67"/>
-      <c r="D4" s="67"/>
-      <c r="E4" s="67"/>
-      <c r="F4" s="67"/>
-      <c r="G4" s="67"/>
-      <c r="H4" s="67"/>
-      <c r="I4" s="67"/>
-      <c r="J4" s="67" t="s">
+      <c r="C4" s="75"/>
+      <c r="D4" s="75"/>
+      <c r="E4" s="75"/>
+      <c r="F4" s="75"/>
+      <c r="G4" s="75"/>
+      <c r="H4" s="75"/>
+      <c r="I4" s="75"/>
+      <c r="J4" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="K4" s="67" t="s">
+      <c r="K4" s="75" t="s">
         <v>11</v>
       </c>
-      <c r="L4" s="67"/>
-      <c r="M4" s="73" t="s">
+      <c r="L4" s="75"/>
+      <c r="M4" s="72" t="s">
         <v>42</v>
       </c>
-      <c r="N4" s="73" t="s">
+      <c r="N4" s="72" t="s">
         <v>10</v>
       </c>
-      <c r="O4" s="67" t="s">
+      <c r="O4" s="75" t="s">
         <v>7</v>
       </c>
       <c r="P4" s="81" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="67" t="s">
+      <c r="Q4" s="75" t="s">
         <v>39</v>
       </c>
-      <c r="R4" s="67" t="s">
+      <c r="R4" s="75" t="s">
         <v>53</v>
       </c>
-      <c r="S4" s="80" t="s">
+      <c r="S4" s="74" t="s">
         <v>54</v>
       </c>
       <c r="T4" s="26"/>
-      <c r="U4" s="67" t="s">
+      <c r="U4" s="75" t="s">
         <v>39</v>
       </c>
-      <c r="V4" s="67" t="s">
+      <c r="V4" s="75" t="s">
         <v>53</v>
       </c>
       <c r="W4" s="45"/>
     </row>
     <row r="5" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="72"/>
+      <c r="A5" s="80"/>
       <c r="B5" s="41" t="s">
         <v>1</v>
       </c>
@@ -3718,23 +3747,23 @@
       <c r="I5" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="67"/>
+      <c r="J5" s="75"/>
       <c r="K5" s="41" t="s">
         <v>12</v>
       </c>
       <c r="L5" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="M5" s="74"/>
-      <c r="N5" s="74"/>
-      <c r="O5" s="67"/>
+      <c r="M5" s="73"/>
+      <c r="N5" s="73"/>
+      <c r="O5" s="75"/>
       <c r="P5" s="81"/>
-      <c r="Q5" s="67"/>
-      <c r="R5" s="67"/>
-      <c r="S5" s="80"/>
+      <c r="Q5" s="75"/>
+      <c r="R5" s="75"/>
+      <c r="S5" s="74"/>
       <c r="T5" s="26"/>
-      <c r="U5" s="67"/>
-      <c r="V5" s="67"/>
+      <c r="U5" s="75"/>
+      <c r="V5" s="75"/>
       <c r="W5" s="45"/>
     </row>
     <row r="6" spans="1:23" s="11" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -3760,7 +3789,7 @@
       <c r="R6" s="37"/>
       <c r="S6" s="3"/>
       <c r="T6" s="40"/>
-      <c r="U6" s="75" t="s">
+      <c r="U6" s="67" t="s">
         <v>18</v>
       </c>
       <c r="V6" s="3" t="s">
@@ -3791,7 +3820,7 @@
       <c r="R7" s="37"/>
       <c r="S7" s="3"/>
       <c r="T7" s="40"/>
-      <c r="U7" s="76"/>
+      <c r="U7" s="68"/>
       <c r="V7" s="3" t="s">
         <v>35</v>
       </c>
@@ -3820,7 +3849,7 @@
       <c r="R8" s="37"/>
       <c r="S8" s="3"/>
       <c r="T8" s="40"/>
-      <c r="U8" s="76"/>
+      <c r="U8" s="68"/>
       <c r="V8" s="3" t="s">
         <v>21</v>
       </c>
@@ -3849,7 +3878,7 @@
       <c r="R9" s="37"/>
       <c r="S9" s="3"/>
       <c r="T9" s="40"/>
-      <c r="U9" s="76"/>
+      <c r="U9" s="68"/>
       <c r="V9" s="3" t="s">
         <v>51</v>
       </c>
@@ -3878,7 +3907,7 @@
       <c r="R10" s="37"/>
       <c r="S10" s="3"/>
       <c r="T10" s="40"/>
-      <c r="U10" s="76"/>
+      <c r="U10" s="68"/>
       <c r="V10" s="3" t="s">
         <v>31</v>
       </c>
@@ -3907,7 +3936,7 @@
       <c r="R11" s="37"/>
       <c r="S11" s="3"/>
       <c r="T11" s="40"/>
-      <c r="U11" s="76"/>
+      <c r="U11" s="68"/>
       <c r="V11" s="3" t="s">
         <v>30</v>
       </c>
@@ -3936,7 +3965,7 @@
       <c r="R12" s="37"/>
       <c r="S12" s="3"/>
       <c r="T12" s="40"/>
-      <c r="U12" s="75" t="s">
+      <c r="U12" s="67" t="s">
         <v>19</v>
       </c>
       <c r="V12" s="3" t="s">
@@ -3967,7 +3996,7 @@
       <c r="R13" s="9"/>
       <c r="S13" s="3"/>
       <c r="T13" s="40"/>
-      <c r="U13" s="76"/>
+      <c r="U13" s="68"/>
       <c r="V13" s="3" t="s">
         <v>37</v>
       </c>
@@ -3996,7 +4025,7 @@
       <c r="R14" s="37"/>
       <c r="S14" s="3"/>
       <c r="T14" s="40"/>
-      <c r="U14" s="76"/>
+      <c r="U14" s="68"/>
       <c r="V14" s="3" t="s">
         <v>36</v>
       </c>
@@ -4025,7 +4054,7 @@
       <c r="R15" s="37"/>
       <c r="S15" s="3"/>
       <c r="T15" s="13"/>
-      <c r="U15" s="76"/>
+      <c r="U15" s="68"/>
       <c r="V15" s="3" t="s">
         <v>24</v>
       </c>
@@ -4054,7 +4083,7 @@
       <c r="R16" s="37"/>
       <c r="S16" s="3"/>
       <c r="T16" s="13"/>
-      <c r="U16" s="77"/>
+      <c r="U16" s="69"/>
       <c r="V16" s="3" t="s">
         <v>25</v>
       </c>
@@ -5285,13 +5314,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="U6:U11"/>
-    <mergeCell ref="U12:U16"/>
-    <mergeCell ref="P4:P5"/>
-    <mergeCell ref="Q4:Q5"/>
-    <mergeCell ref="R4:R5"/>
-    <mergeCell ref="S4:S5"/>
-    <mergeCell ref="U4:U5"/>
     <mergeCell ref="V4:V5"/>
     <mergeCell ref="A1:V1"/>
     <mergeCell ref="A2:D2"/>
@@ -5303,6 +5325,13 @@
     <mergeCell ref="M4:M5"/>
     <mergeCell ref="N4:N5"/>
     <mergeCell ref="O4:O5"/>
+    <mergeCell ref="U6:U11"/>
+    <mergeCell ref="U12:U16"/>
+    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="Q4:Q5"/>
+    <mergeCell ref="R4:R5"/>
+    <mergeCell ref="S4:S5"/>
+    <mergeCell ref="U4:U5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
anh tuan bg + lap dat
</commit_message>
<xml_diff>
--- a/5. WS/1. Bộ phận bảo hành/1. Thực hiện sửa chữa bảo hành/nam2022/Thang11/2.XulyBH/XLBH2211_AnhTuanBG.xlsx
+++ b/5. WS/1. Bộ phận bảo hành/1. Thực hiện sửa chữa bảo hành/nam2022/Thang11/2.XulyBH/XLBH2211_AnhTuanBG.xlsx
@@ -727,6 +727,30 @@
     <xf numFmtId="1" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -742,32 +766,8 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1078,8 +1078,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X115"/>
   <sheetViews>
-    <sheetView showZeros="0" tabSelected="1" topLeftCell="L1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="S17" sqref="S17"/>
+    <sheetView showZeros="0" tabSelected="1" topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1111,41 +1111,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="76"/>
-      <c r="B1" s="76"/>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
-      <c r="F1" s="76"/>
-      <c r="G1" s="76"/>
-      <c r="H1" s="76"/>
-      <c r="I1" s="76"/>
-      <c r="J1" s="76"/>
-      <c r="K1" s="76"/>
-      <c r="L1" s="76"/>
-      <c r="M1" s="76"/>
-      <c r="N1" s="76"/>
-      <c r="O1" s="76"/>
-      <c r="P1" s="76"/>
-      <c r="Q1" s="76"/>
-      <c r="R1" s="76"/>
-      <c r="S1" s="76"/>
-      <c r="T1" s="76"/>
-      <c r="U1" s="76"/>
-      <c r="V1" s="76"/>
+      <c r="A1" s="68"/>
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="68"/>
+      <c r="J1" s="68"/>
+      <c r="K1" s="68"/>
+      <c r="L1" s="68"/>
+      <c r="M1" s="68"/>
+      <c r="N1" s="68"/>
+      <c r="O1" s="68"/>
+      <c r="P1" s="68"/>
+      <c r="Q1" s="68"/>
+      <c r="R1" s="68"/>
+      <c r="S1" s="68"/>
+      <c r="T1" s="68"/>
+      <c r="U1" s="68"/>
+      <c r="V1" s="68"/>
       <c r="W1" s="44"/>
     </row>
     <row r="2" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="77" t="s">
+      <c r="A2" s="69" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="78"/>
-      <c r="C2" s="78"/>
-      <c r="D2" s="78"/>
-      <c r="E2" s="79" t="s">
+      <c r="B2" s="70"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="71" t="s">
         <v>63</v>
       </c>
-      <c r="F2" s="79"/>
+      <c r="F2" s="71"/>
       <c r="G2" s="4"/>
       <c r="H2" s="20"/>
       <c r="I2" s="48"/>
@@ -1190,58 +1190,58 @@
       <c r="W3" s="26"/>
     </row>
     <row r="4" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="80" t="s">
+      <c r="A4" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="75" t="s">
+      <c r="B4" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="75"/>
-      <c r="D4" s="75"/>
-      <c r="E4" s="75"/>
-      <c r="F4" s="75"/>
-      <c r="G4" s="75"/>
-      <c r="H4" s="75"/>
-      <c r="I4" s="75"/>
-      <c r="J4" s="75" t="s">
+      <c r="C4" s="67"/>
+      <c r="D4" s="67"/>
+      <c r="E4" s="67"/>
+      <c r="F4" s="67"/>
+      <c r="G4" s="67"/>
+      <c r="H4" s="67"/>
+      <c r="I4" s="67"/>
+      <c r="J4" s="67" t="s">
         <v>6</v>
       </c>
-      <c r="K4" s="75" t="s">
+      <c r="K4" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="L4" s="75"/>
-      <c r="M4" s="72" t="s">
+      <c r="L4" s="67"/>
+      <c r="M4" s="73" t="s">
         <v>42</v>
       </c>
-      <c r="N4" s="72" t="s">
+      <c r="N4" s="73" t="s">
         <v>10</v>
       </c>
-      <c r="O4" s="72" t="s">
+      <c r="O4" s="73" t="s">
         <v>7</v>
       </c>
-      <c r="P4" s="70" t="s">
+      <c r="P4" s="78" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="72" t="s">
+      <c r="Q4" s="73" t="s">
         <v>39</v>
       </c>
-      <c r="R4" s="72" t="s">
+      <c r="R4" s="73" t="s">
         <v>53</v>
       </c>
-      <c r="S4" s="74" t="s">
+      <c r="S4" s="80" t="s">
         <v>54</v>
       </c>
       <c r="T4" s="26"/>
-      <c r="U4" s="75" t="s">
+      <c r="U4" s="67" t="s">
         <v>39</v>
       </c>
-      <c r="V4" s="75" t="s">
+      <c r="V4" s="67" t="s">
         <v>53</v>
       </c>
       <c r="W4" s="45"/>
     </row>
     <row r="5" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="80"/>
+      <c r="A5" s="72"/>
       <c r="B5" s="56" t="s">
         <v>1</v>
       </c>
@@ -1266,23 +1266,23 @@
       <c r="I5" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="75"/>
+      <c r="J5" s="67"/>
       <c r="K5" s="56" t="s">
         <v>12</v>
       </c>
       <c r="L5" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="M5" s="73"/>
-      <c r="N5" s="73"/>
-      <c r="O5" s="73"/>
-      <c r="P5" s="71"/>
-      <c r="Q5" s="73"/>
-      <c r="R5" s="73"/>
-      <c r="S5" s="74"/>
+      <c r="M5" s="74"/>
+      <c r="N5" s="74"/>
+      <c r="O5" s="74"/>
+      <c r="P5" s="79"/>
+      <c r="Q5" s="74"/>
+      <c r="R5" s="74"/>
+      <c r="S5" s="80"/>
       <c r="T5" s="26"/>
-      <c r="U5" s="75"/>
-      <c r="V5" s="75"/>
+      <c r="U5" s="67"/>
+      <c r="V5" s="67"/>
       <c r="W5" s="45"/>
     </row>
     <row r="6" spans="1:23" s="11" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1338,7 +1338,7 @@
       </c>
       <c r="S6" s="64"/>
       <c r="T6" s="55"/>
-      <c r="U6" s="67" t="s">
+      <c r="U6" s="75" t="s">
         <v>18</v>
       </c>
       <c r="V6" s="3" t="s">
@@ -1399,7 +1399,7 @@
       </c>
       <c r="S7" s="64"/>
       <c r="T7" s="55"/>
-      <c r="U7" s="68"/>
+      <c r="U7" s="76"/>
       <c r="V7" s="3" t="s">
         <v>35</v>
       </c>
@@ -1458,7 +1458,7 @@
       </c>
       <c r="S8" s="64"/>
       <c r="T8" s="55"/>
-      <c r="U8" s="68"/>
+      <c r="U8" s="76"/>
       <c r="V8" s="3" t="s">
         <v>21</v>
       </c>
@@ -1517,7 +1517,7 @@
       </c>
       <c r="S9" s="64"/>
       <c r="T9" s="55"/>
-      <c r="U9" s="68"/>
+      <c r="U9" s="76"/>
       <c r="V9" s="3" t="s">
         <v>51</v>
       </c>
@@ -1578,7 +1578,7 @@
       </c>
       <c r="S10" s="64"/>
       <c r="T10" s="55"/>
-      <c r="U10" s="68"/>
+      <c r="U10" s="76"/>
       <c r="V10" s="3" t="s">
         <v>31</v>
       </c>
@@ -1637,7 +1637,7 @@
       </c>
       <c r="S11" s="64"/>
       <c r="T11" s="55"/>
-      <c r="U11" s="68"/>
+      <c r="U11" s="76"/>
       <c r="V11" s="3" t="s">
         <v>30</v>
       </c>
@@ -1696,7 +1696,7 @@
       </c>
       <c r="S12" s="64"/>
       <c r="T12" s="55"/>
-      <c r="U12" s="67" t="s">
+      <c r="U12" s="75" t="s">
         <v>19</v>
       </c>
       <c r="V12" s="3" t="s">
@@ -1727,7 +1727,7 @@
       <c r="R13" s="61"/>
       <c r="S13" s="64"/>
       <c r="T13" s="55"/>
-      <c r="U13" s="68"/>
+      <c r="U13" s="76"/>
       <c r="V13" s="3" t="s">
         <v>37</v>
       </c>
@@ -1756,7 +1756,7 @@
       <c r="R14" s="61"/>
       <c r="S14" s="64"/>
       <c r="T14" s="55"/>
-      <c r="U14" s="68"/>
+      <c r="U14" s="76"/>
       <c r="V14" s="3" t="s">
         <v>36</v>
       </c>
@@ -1785,7 +1785,7 @@
       <c r="R15" s="61"/>
       <c r="S15" s="64"/>
       <c r="T15" s="13"/>
-      <c r="U15" s="68"/>
+      <c r="U15" s="76"/>
       <c r="V15" s="3" t="s">
         <v>24</v>
       </c>
@@ -1814,7 +1814,7 @@
       <c r="R16" s="61"/>
       <c r="S16" s="64"/>
       <c r="T16" s="13"/>
-      <c r="U16" s="69"/>
+      <c r="U16" s="77"/>
       <c r="V16" s="3" t="s">
         <v>25</v>
       </c>
@@ -3531,6 +3531,13 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="U6:U11"/>
+    <mergeCell ref="U12:U16"/>
+    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="Q4:Q5"/>
+    <mergeCell ref="R4:R5"/>
+    <mergeCell ref="S4:S5"/>
+    <mergeCell ref="U4:U5"/>
     <mergeCell ref="V4:V5"/>
     <mergeCell ref="A1:V1"/>
     <mergeCell ref="A2:D2"/>
@@ -3542,13 +3549,6 @@
     <mergeCell ref="M4:M5"/>
     <mergeCell ref="N4:N5"/>
     <mergeCell ref="O4:O5"/>
-    <mergeCell ref="U6:U11"/>
-    <mergeCell ref="U12:U16"/>
-    <mergeCell ref="P4:P5"/>
-    <mergeCell ref="Q4:Q5"/>
-    <mergeCell ref="R4:R5"/>
-    <mergeCell ref="S4:S5"/>
-    <mergeCell ref="U4:U5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3592,41 +3592,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="76"/>
-      <c r="B1" s="76"/>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
-      <c r="F1" s="76"/>
-      <c r="G1" s="76"/>
-      <c r="H1" s="76"/>
-      <c r="I1" s="76"/>
-      <c r="J1" s="76"/>
-      <c r="K1" s="76"/>
-      <c r="L1" s="76"/>
-      <c r="M1" s="76"/>
-      <c r="N1" s="76"/>
-      <c r="O1" s="76"/>
-      <c r="P1" s="76"/>
-      <c r="Q1" s="76"/>
-      <c r="R1" s="76"/>
-      <c r="S1" s="76"/>
-      <c r="T1" s="76"/>
-      <c r="U1" s="76"/>
-      <c r="V1" s="76"/>
+      <c r="A1" s="68"/>
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="68"/>
+      <c r="J1" s="68"/>
+      <c r="K1" s="68"/>
+      <c r="L1" s="68"/>
+      <c r="M1" s="68"/>
+      <c r="N1" s="68"/>
+      <c r="O1" s="68"/>
+      <c r="P1" s="68"/>
+      <c r="Q1" s="68"/>
+      <c r="R1" s="68"/>
+      <c r="S1" s="68"/>
+      <c r="T1" s="68"/>
+      <c r="U1" s="68"/>
+      <c r="V1" s="68"/>
       <c r="W1" s="44"/>
     </row>
     <row r="2" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="77" t="s">
+      <c r="A2" s="69" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="78"/>
-      <c r="C2" s="78"/>
-      <c r="D2" s="78"/>
-      <c r="E2" s="79" t="s">
+      <c r="B2" s="70"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="71" t="s">
         <v>63</v>
       </c>
-      <c r="F2" s="79"/>
+      <c r="F2" s="71"/>
       <c r="G2" s="4"/>
       <c r="H2" s="20"/>
       <c r="I2" s="20"/>
@@ -3671,58 +3671,58 @@
       <c r="W3" s="26"/>
     </row>
     <row r="4" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="80" t="s">
+      <c r="A4" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="75" t="s">
+      <c r="B4" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="75"/>
-      <c r="D4" s="75"/>
-      <c r="E4" s="75"/>
-      <c r="F4" s="75"/>
-      <c r="G4" s="75"/>
-      <c r="H4" s="75"/>
-      <c r="I4" s="75"/>
-      <c r="J4" s="75" t="s">
+      <c r="C4" s="67"/>
+      <c r="D4" s="67"/>
+      <c r="E4" s="67"/>
+      <c r="F4" s="67"/>
+      <c r="G4" s="67"/>
+      <c r="H4" s="67"/>
+      <c r="I4" s="67"/>
+      <c r="J4" s="67" t="s">
         <v>6</v>
       </c>
-      <c r="K4" s="75" t="s">
+      <c r="K4" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="L4" s="75"/>
-      <c r="M4" s="72" t="s">
+      <c r="L4" s="67"/>
+      <c r="M4" s="73" t="s">
         <v>42</v>
       </c>
-      <c r="N4" s="72" t="s">
+      <c r="N4" s="73" t="s">
         <v>10</v>
       </c>
-      <c r="O4" s="75" t="s">
+      <c r="O4" s="67" t="s">
         <v>7</v>
       </c>
       <c r="P4" s="81" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="75" t="s">
+      <c r="Q4" s="67" t="s">
         <v>39</v>
       </c>
-      <c r="R4" s="75" t="s">
+      <c r="R4" s="67" t="s">
         <v>53</v>
       </c>
-      <c r="S4" s="74" t="s">
+      <c r="S4" s="80" t="s">
         <v>54</v>
       </c>
       <c r="T4" s="26"/>
-      <c r="U4" s="75" t="s">
+      <c r="U4" s="67" t="s">
         <v>39</v>
       </c>
-      <c r="V4" s="75" t="s">
+      <c r="V4" s="67" t="s">
         <v>53</v>
       </c>
       <c r="W4" s="45"/>
     </row>
     <row r="5" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="80"/>
+      <c r="A5" s="72"/>
       <c r="B5" s="41" t="s">
         <v>1</v>
       </c>
@@ -3747,23 +3747,23 @@
       <c r="I5" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="75"/>
+      <c r="J5" s="67"/>
       <c r="K5" s="41" t="s">
         <v>12</v>
       </c>
       <c r="L5" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="M5" s="73"/>
-      <c r="N5" s="73"/>
-      <c r="O5" s="75"/>
+      <c r="M5" s="74"/>
+      <c r="N5" s="74"/>
+      <c r="O5" s="67"/>
       <c r="P5" s="81"/>
-      <c r="Q5" s="75"/>
-      <c r="R5" s="75"/>
-      <c r="S5" s="74"/>
+      <c r="Q5" s="67"/>
+      <c r="R5" s="67"/>
+      <c r="S5" s="80"/>
       <c r="T5" s="26"/>
-      <c r="U5" s="75"/>
-      <c r="V5" s="75"/>
+      <c r="U5" s="67"/>
+      <c r="V5" s="67"/>
       <c r="W5" s="45"/>
     </row>
     <row r="6" spans="1:23" s="11" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -3789,7 +3789,7 @@
       <c r="R6" s="37"/>
       <c r="S6" s="3"/>
       <c r="T6" s="40"/>
-      <c r="U6" s="67" t="s">
+      <c r="U6" s="75" t="s">
         <v>18</v>
       </c>
       <c r="V6" s="3" t="s">
@@ -3820,7 +3820,7 @@
       <c r="R7" s="37"/>
       <c r="S7" s="3"/>
       <c r="T7" s="40"/>
-      <c r="U7" s="68"/>
+      <c r="U7" s="76"/>
       <c r="V7" s="3" t="s">
         <v>35</v>
       </c>
@@ -3849,7 +3849,7 @@
       <c r="R8" s="37"/>
       <c r="S8" s="3"/>
       <c r="T8" s="40"/>
-      <c r="U8" s="68"/>
+      <c r="U8" s="76"/>
       <c r="V8" s="3" t="s">
         <v>21</v>
       </c>
@@ -3878,7 +3878,7 @@
       <c r="R9" s="37"/>
       <c r="S9" s="3"/>
       <c r="T9" s="40"/>
-      <c r="U9" s="68"/>
+      <c r="U9" s="76"/>
       <c r="V9" s="3" t="s">
         <v>51</v>
       </c>
@@ -3907,7 +3907,7 @@
       <c r="R10" s="37"/>
       <c r="S10" s="3"/>
       <c r="T10" s="40"/>
-      <c r="U10" s="68"/>
+      <c r="U10" s="76"/>
       <c r="V10" s="3" t="s">
         <v>31</v>
       </c>
@@ -3936,7 +3936,7 @@
       <c r="R11" s="37"/>
       <c r="S11" s="3"/>
       <c r="T11" s="40"/>
-      <c r="U11" s="68"/>
+      <c r="U11" s="76"/>
       <c r="V11" s="3" t="s">
         <v>30</v>
       </c>
@@ -3965,7 +3965,7 @@
       <c r="R12" s="37"/>
       <c r="S12" s="3"/>
       <c r="T12" s="40"/>
-      <c r="U12" s="67" t="s">
+      <c r="U12" s="75" t="s">
         <v>19</v>
       </c>
       <c r="V12" s="3" t="s">
@@ -3996,7 +3996,7 @@
       <c r="R13" s="9"/>
       <c r="S13" s="3"/>
       <c r="T13" s="40"/>
-      <c r="U13" s="68"/>
+      <c r="U13" s="76"/>
       <c r="V13" s="3" t="s">
         <v>37</v>
       </c>
@@ -4025,7 +4025,7 @@
       <c r="R14" s="37"/>
       <c r="S14" s="3"/>
       <c r="T14" s="40"/>
-      <c r="U14" s="68"/>
+      <c r="U14" s="76"/>
       <c r="V14" s="3" t="s">
         <v>36</v>
       </c>
@@ -4054,7 +4054,7 @@
       <c r="R15" s="37"/>
       <c r="S15" s="3"/>
       <c r="T15" s="13"/>
-      <c r="U15" s="68"/>
+      <c r="U15" s="76"/>
       <c r="V15" s="3" t="s">
         <v>24</v>
       </c>
@@ -4083,7 +4083,7 @@
       <c r="R16" s="37"/>
       <c r="S16" s="3"/>
       <c r="T16" s="13"/>
-      <c r="U16" s="69"/>
+      <c r="U16" s="77"/>
       <c r="V16" s="3" t="s">
         <v>25</v>
       </c>
@@ -5314,6 +5314,13 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="U6:U11"/>
+    <mergeCell ref="U12:U16"/>
+    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="Q4:Q5"/>
+    <mergeCell ref="R4:R5"/>
+    <mergeCell ref="S4:S5"/>
+    <mergeCell ref="U4:U5"/>
     <mergeCell ref="V4:V5"/>
     <mergeCell ref="A1:V1"/>
     <mergeCell ref="A2:D2"/>
@@ -5325,13 +5332,6 @@
     <mergeCell ref="M4:M5"/>
     <mergeCell ref="N4:N5"/>
     <mergeCell ref="O4:O5"/>
-    <mergeCell ref="U6:U11"/>
-    <mergeCell ref="U12:U16"/>
-    <mergeCell ref="P4:P5"/>
-    <mergeCell ref="Q4:Q5"/>
-    <mergeCell ref="R4:R5"/>
-    <mergeCell ref="S4:S5"/>
-    <mergeCell ref="U4:U5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>